<commit_message>
changed the name of the dataset to GHI
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/IFPRI-GHI/IFPRI-GHI-Child_Mortality.xlsx
+++ b/Simple_XLS_Importer/data/IFPRI-GHI/IFPRI-GHI-Child_Mortality.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="525" windowWidth="17415" windowHeight="5835"/>
+    <workbookView xWindow="750" yWindow="525" windowWidth="17415" windowHeight="5835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="3" r:id="rId1"/>
     <sheet name="metadata" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -383,9 +383,6 @@
     <t>IFPRI</t>
   </si>
   <si>
-    <t>DAT-0</t>
-  </si>
-  <si>
     <t>LBY</t>
   </si>
   <si>
@@ -426,6 +423,9 @@
   </si>
   <si>
     <t>GHI-Child_Mortality</t>
+  </si>
+  <si>
+    <t>GHI</t>
   </si>
 </sst>
 </file>
@@ -803,7 +803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="C28" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
@@ -825,7 +825,7 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" s="3">
         <v>2015</v>
@@ -836,7 +836,7 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" s="3">
         <v>1990</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4" s="3">
         <v>1995</v>
@@ -858,7 +858,7 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" s="3">
         <v>2000</v>
@@ -869,7 +869,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6" s="3">
         <v>2005</v>
@@ -1232,7 +1232,7 @@
     </row>
     <row r="39" spans="1:3" ht="12.75">
       <c r="A39" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B39" s="3">
         <v>2015</v>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="40" spans="1:3" ht="12.75">
       <c r="A40" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B40" s="3">
         <v>1990</v>
@@ -1254,7 +1254,7 @@
     </row>
     <row r="41" spans="1:3" ht="12.75">
       <c r="A41" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B41" s="3">
         <v>1995</v>
@@ -1265,7 +1265,7 @@
     </row>
     <row r="42" spans="1:3" ht="12.75">
       <c r="A42" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B42" s="3">
         <v>2000</v>
@@ -1276,7 +1276,7 @@
     </row>
     <row r="43" spans="1:3" ht="12.75">
       <c r="A43" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B43" s="3">
         <v>2005</v>
@@ -1441,7 +1441,7 @@
     </row>
     <row r="58" spans="1:3" ht="12.75">
       <c r="A58" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B58" s="3">
         <v>2015</v>
@@ -1452,7 +1452,7 @@
     </row>
     <row r="59" spans="1:3" ht="12.75">
       <c r="A59" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B59" s="3">
         <v>1990</v>
@@ -1463,7 +1463,7 @@
     </row>
     <row r="60" spans="1:3" ht="12.75">
       <c r="A60" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B60" s="3">
         <v>1995</v>
@@ -1474,7 +1474,7 @@
     </row>
     <row r="61" spans="1:3" ht="12.75">
       <c r="A61" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B61" s="3">
         <v>2000</v>
@@ -1485,7 +1485,7 @@
     </row>
     <row r="62" spans="1:3" ht="12.75">
       <c r="A62" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B62" s="3">
         <v>2005</v>
@@ -1804,7 +1804,7 @@
     </row>
     <row r="91" spans="1:3" ht="12.75">
       <c r="A91" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B91" s="3">
         <v>2015</v>
@@ -1815,7 +1815,7 @@
     </row>
     <row r="92" spans="1:3" ht="12.75">
       <c r="A92" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B92" s="3">
         <v>1990</v>
@@ -1826,7 +1826,7 @@
     </row>
     <row r="93" spans="1:3" ht="12.75">
       <c r="A93" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B93" s="3">
         <v>1995</v>
@@ -1837,7 +1837,7 @@
     </row>
     <row r="94" spans="1:3" ht="12.75">
       <c r="A94" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B94" s="3">
         <v>2000</v>
@@ -1848,7 +1848,7 @@
     </row>
     <row r="95" spans="1:3" ht="12.75">
       <c r="A95" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B95" s="3">
         <v>2005</v>
@@ -2233,7 +2233,7 @@
     </row>
     <row r="130" spans="1:3" ht="12.75">
       <c r="A130" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B130" s="3">
         <v>2015</v>
@@ -2244,7 +2244,7 @@
     </row>
     <row r="131" spans="1:3" ht="12.75">
       <c r="A131" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B131" s="3">
         <v>1990</v>
@@ -2255,7 +2255,7 @@
     </row>
     <row r="132" spans="1:3" ht="12.75">
       <c r="A132" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B132" s="3">
         <v>1995</v>
@@ -2266,7 +2266,7 @@
     </row>
     <row r="133" spans="1:3" ht="12.75">
       <c r="A133" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B133" s="3">
         <v>2000</v>
@@ -2277,7 +2277,7 @@
     </row>
     <row r="134" spans="1:3" ht="12.75">
       <c r="A134" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B134" s="3">
         <v>2005</v>
@@ -2563,7 +2563,7 @@
     </row>
     <row r="160" spans="1:3" ht="12.75">
       <c r="A160" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B160" s="3">
         <v>2015</v>
@@ -2574,7 +2574,7 @@
     </row>
     <row r="161" spans="1:3" ht="12.75">
       <c r="A161" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B161" s="3">
         <v>1990</v>
@@ -2585,7 +2585,7 @@
     </row>
     <row r="162" spans="1:3" ht="12.75">
       <c r="A162" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B162" s="3">
         <v>1995</v>
@@ -2596,7 +2596,7 @@
     </row>
     <row r="163" spans="1:3" ht="12.75">
       <c r="A163" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B163" s="3">
         <v>2000</v>
@@ -2607,7 +2607,7 @@
     </row>
     <row r="164" spans="1:3" ht="12.75">
       <c r="A164" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B164" s="3">
         <v>2005</v>
@@ -2860,7 +2860,7 @@
     </row>
     <row r="187" spans="1:3" ht="12.75">
       <c r="A187" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B187" s="3">
         <v>1995</v>
@@ -2871,7 +2871,7 @@
     </row>
     <row r="188" spans="1:3" ht="12.75">
       <c r="A188" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B188" s="3">
         <v>2000</v>
@@ -5280,7 +5280,7 @@
     </row>
     <row r="407" spans="1:3" ht="12.75">
       <c r="A407" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B407" s="3">
         <v>2015</v>
@@ -5291,7 +5291,7 @@
     </row>
     <row r="408" spans="1:3" ht="12.75">
       <c r="A408" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B408" s="3">
         <v>1990</v>
@@ -5302,7 +5302,7 @@
     </row>
     <row r="409" spans="1:3" ht="12.75">
       <c r="A409" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B409" s="3">
         <v>1995</v>
@@ -5313,7 +5313,7 @@
     </row>
     <row r="410" spans="1:3" ht="12.75">
       <c r="A410" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B410" s="3">
         <v>2000</v>
@@ -5324,7 +5324,7 @@
     </row>
     <row r="411" spans="1:3" ht="12.75">
       <c r="A411" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B411" s="3">
         <v>2005</v>
@@ -5456,7 +5456,7 @@
     </row>
     <row r="423" spans="1:3" ht="12.75">
       <c r="A423" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B423" s="3">
         <v>2015</v>
@@ -5467,7 +5467,7 @@
     </row>
     <row r="424" spans="1:3" ht="12.75">
       <c r="A424" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B424" s="3">
         <v>1990</v>
@@ -5478,7 +5478,7 @@
     </row>
     <row r="425" spans="1:3" ht="12.75">
       <c r="A425" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B425" s="3">
         <v>1995</v>
@@ -5489,7 +5489,7 @@
     </row>
     <row r="426" spans="1:3" ht="12.75">
       <c r="A426" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B426" s="3">
         <v>2000</v>
@@ -5885,7 +5885,7 @@
     </row>
     <row r="462" spans="1:3" ht="12.75">
       <c r="A462" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B462" s="3">
         <v>2015</v>
@@ -5896,7 +5896,7 @@
     </row>
     <row r="463" spans="1:3" ht="12.75">
       <c r="A463" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B463" s="3">
         <v>1990</v>
@@ -5907,7 +5907,7 @@
     </row>
     <row r="464" spans="1:3" ht="12.75">
       <c r="A464" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B464" s="3">
         <v>1995</v>
@@ -5918,7 +5918,7 @@
     </row>
     <row r="465" spans="1:3" ht="12.75">
       <c r="A465" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B465" s="3">
         <v>2000</v>
@@ -5929,7 +5929,7 @@
     </row>
     <row r="466" spans="1:3" ht="12.75">
       <c r="A466" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B466" s="3">
         <v>2005</v>
@@ -5940,7 +5940,7 @@
     </row>
     <row r="467" spans="1:3" ht="12.75">
       <c r="A467" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B467" s="3">
         <v>2015</v>
@@ -5984,7 +5984,7 @@
     </row>
     <row r="471" spans="1:3" ht="12.75">
       <c r="A471" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B471" s="3">
         <v>2015</v>
@@ -6083,7 +6083,7 @@
     </row>
     <row r="480" spans="1:3" ht="12.75">
       <c r="A480" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B480" s="3">
         <v>2015</v>
@@ -6094,7 +6094,7 @@
     </row>
     <row r="481" spans="1:3" ht="12.75">
       <c r="A481" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B481" s="3">
         <v>1990</v>
@@ -6105,7 +6105,7 @@
     </row>
     <row r="482" spans="1:3" ht="12.75">
       <c r="A482" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B482" s="3">
         <v>2000</v>
@@ -6116,7 +6116,7 @@
     </row>
     <row r="483" spans="1:3" ht="12.75">
       <c r="A483" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B483" s="3">
         <v>2005</v>
@@ -8052,8 +8052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -8075,7 +8075,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -8083,7 +8083,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>